<commit_message>
Final Form of announcement
</commit_message>
<xml_diff>
--- a/Data/kosdaq/table6.xlsx
+++ b/Data/kosdaq/table6.xlsx
@@ -423,10 +423,10 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>4475</v>
+        <v>831</v>
       </c>
       <c r="D2">
-        <v>4598</v>
+        <v>863</v>
       </c>
       <c r="E2">
         <v>0.49</v>
@@ -438,13 +438,13 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1147</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>1203</v>
       </c>
       <c r="E3">
-        <v>0.4</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -453,13 +453,10 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>67</v>
-      </c>
-      <c r="E4">
-        <v>0.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -468,13 +465,13 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>906</v>
+        <v>1519</v>
       </c>
       <c r="D5">
-        <v>854</v>
+        <v>1523</v>
       </c>
       <c r="E5">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -483,13 +480,13 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>1940</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>1944</v>
       </c>
       <c r="E6">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:5">

</xml_diff>